<commit_message>
Corrections on CAPI and some syntax from ToT
We did some corrections on comments stated/found from  ToT on Listing, Community and Household questionnaires.
</commit_message>
<xml_diff>
--- a/LookupFiles/users.xlsx
+++ b/LookupFiles/users.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/699cb0a564aebff5/Documents/GitHub/ENERGY/LookupFiles/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\ENERGY\LookupFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{63C9E6FD-D71F-4A94-A523-53645D746227}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{02E49AF5-2916-4D3E-A1D2-77DF47C05AF3}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34E614DA-5905-49B3-9302-6F55D9001BD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{E83E24DF-ECF9-4033-ACEC-B0F7094A083B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{E83E24DF-ECF9-4033-ACEC-B0F7094A083B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="44">
   <si>
     <t>Login</t>
   </si>
@@ -133,16 +133,46 @@
   </si>
   <si>
     <t>Ramadhani Kalinga</t>
+  </si>
+  <si>
+    <t>shamimu</t>
+  </si>
+  <si>
+    <t>eline</t>
+  </si>
+  <si>
+    <t>joshua</t>
+  </si>
+  <si>
+    <t>lightness</t>
+  </si>
+  <si>
+    <t>Interview 01</t>
+  </si>
+  <si>
+    <t>Interview 02</t>
+  </si>
+  <si>
+    <t>Interview 03</t>
+  </si>
+  <si>
+    <t>Interview 04</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -484,20 +514,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A43E83A9-4175-4444-8AB1-9925632E1DE6}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="3" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -514,7 +544,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -528,7 +558,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -545,7 +575,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -559,7 +589,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -573,7 +603,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -587,7 +617,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -598,7 +628,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -612,7 +642,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -629,7 +659,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -643,7 +673,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -657,7 +687,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -674,7 +704,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -691,7 +721,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -708,7 +738,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -725,7 +755,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -739,7 +769,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>25</v>
       </c>
@@ -756,7 +786,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>26</v>
       </c>
@@ -773,7 +803,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -790,7 +820,76 @@
         <v>35</v>
       </c>
     </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20">
+        <v>5</v>
+      </c>
+      <c r="C20">
+        <v>800</v>
+      </c>
+      <c r="D20" t="s">
+        <v>18</v>
+      </c>
+      <c r="E20" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21">
+        <v>5</v>
+      </c>
+      <c r="C21">
+        <v>900</v>
+      </c>
+      <c r="D21" t="s">
+        <v>18</v>
+      </c>
+      <c r="E21" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22">
+        <v>5</v>
+      </c>
+      <c r="C22">
+        <v>850</v>
+      </c>
+      <c r="D22" t="s">
+        <v>18</v>
+      </c>
+      <c r="E22" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23">
+        <v>5</v>
+      </c>
+      <c r="C23">
+        <v>950</v>
+      </c>
+      <c r="D23" t="s">
+        <v>18</v>
+      </c>
+      <c r="E23" t="s">
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changed users to max 10 character logins
</commit_message>
<xml_diff>
--- a/LookupFiles/users.xlsx
+++ b/LookupFiles/users.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SSB\ENERGY\LookupFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\ENERGY\LookupFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1238BE0-E0A4-4925-97BF-17E9695BBD53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10296"/>
+    <workbookView xWindow="3465" yWindow="1350" windowWidth="21600" windowHeight="13500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -269,18 +270,12 @@
     <t>wwilson</t>
   </si>
   <si>
-    <t>lalojamento</t>
-  </si>
-  <si>
     <t>apentear</t>
   </si>
   <si>
     <t>rraquito</t>
   </si>
   <si>
-    <t>gmuandipezar</t>
-  </si>
-  <si>
     <t>hticha</t>
   </si>
   <si>
@@ -311,9 +306,6 @@
     <t>zluis</t>
   </si>
   <si>
-    <t>jvilanculos</t>
-  </si>
-  <si>
     <t>jchissano</t>
   </si>
   <si>
@@ -357,12 +349,21 @@
   </si>
   <si>
     <t>amawai</t>
+  </si>
+  <si>
+    <t>lino</t>
+  </si>
+  <si>
+    <t>graca</t>
+  </si>
+  <si>
+    <t>jonas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -848,22 +849,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E45" sqref="E45"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="8.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="42.5546875" customWidth="1"/>
+    <col min="1" max="1" width="19.5703125" customWidth="1"/>
+    <col min="2" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -880,12 +881,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>57</v>
       </c>
       <c r="B2" s="7">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="7" t="s">
@@ -895,7 +896,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>58</v>
       </c>
@@ -912,7 +913,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="19.2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>59</v>
       </c>
@@ -929,7 +930,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>60</v>
       </c>
@@ -946,12 +947,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>61</v>
       </c>
       <c r="B6" s="7">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="7" t="s">
@@ -961,7 +962,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>62</v>
       </c>
@@ -978,7 +979,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>63</v>
       </c>
@@ -995,7 +996,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>64</v>
       </c>
@@ -1012,7 +1013,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>65</v>
       </c>
@@ -1027,7 +1028,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>66</v>
       </c>
@@ -1044,7 +1045,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
         <v>67</v>
       </c>
@@ -1061,7 +1062,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
         <v>68</v>
       </c>
@@ -1078,7 +1079,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>69</v>
       </c>
@@ -1093,9 +1094,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B15" s="4">
         <v>4</v>
@@ -1107,10 +1108,10 @@
         <v>6</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
         <v>70</v>
       </c>
@@ -1127,7 +1128,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
         <v>71</v>
       </c>
@@ -1144,7 +1145,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>72</v>
       </c>
@@ -1159,7 +1160,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>73</v>
       </c>
@@ -1176,7 +1177,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>74</v>
       </c>
@@ -1193,7 +1194,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>75</v>
       </c>
@@ -1210,7 +1211,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>76</v>
       </c>
@@ -1225,7 +1226,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>77</v>
       </c>
@@ -1242,7 +1243,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>78</v>
       </c>
@@ -1259,7 +1260,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>79</v>
       </c>
@@ -1276,7 +1277,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>80</v>
       </c>
@@ -1291,9 +1292,9 @@
         <v>41</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>81</v>
+        <v>108</v>
       </c>
       <c r="B27" s="4">
         <v>7</v>
@@ -1308,9 +1309,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B28" s="4">
         <v>7</v>
@@ -1325,9 +1326,9 @@
         <v>42</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B29" s="4">
         <v>7</v>
@@ -1342,9 +1343,9 @@
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>84</v>
+        <v>109</v>
       </c>
       <c r="B30" s="7">
         <v>8</v>
@@ -1357,9 +1358,9 @@
         <v>43</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B31" s="4">
         <v>8</v>
@@ -1374,9 +1375,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B32" s="4">
         <v>8</v>
@@ -1391,9 +1392,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B33" s="4">
         <v>8</v>
@@ -1408,9 +1409,9 @@
         <v>44</v>
       </c>
     </row>
-    <row r="34" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B34" s="7">
         <v>9</v>
@@ -1423,9 +1424,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B35" s="4">
         <v>9</v>
@@ -1440,9 +1441,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B36" s="4">
         <v>9</v>
@@ -1457,9 +1458,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B37" s="4">
         <v>9</v>
@@ -1474,9 +1475,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="38" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B38" s="7">
         <v>10</v>
@@ -1489,9 +1490,9 @@
         <v>46</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B39" s="4">
         <v>10</v>
@@ -1506,9 +1507,9 @@
         <v>23</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B40" s="4">
         <v>10</v>
@@ -1523,9 +1524,9 @@
         <v>31</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>95</v>
+        <v>110</v>
       </c>
       <c r="B41" s="4">
         <v>10</v>
@@ -1540,9 +1541,9 @@
         <v>47</v>
       </c>
     </row>
-    <row r="42" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B42" s="7">
         <v>11</v>
@@ -1555,9 +1556,9 @@
         <v>48</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B43" s="4">
         <v>11</v>
@@ -1569,12 +1570,12 @@
         <v>6</v>
       </c>
       <c r="E43" s="11" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B44" s="4">
         <v>11</v>
@@ -1589,9 +1590,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B45" s="4">
         <v>11</v>
@@ -1606,9 +1607,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="46" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B46" s="7">
         <v>11</v>
@@ -1621,9 +1622,9 @@
         <v>49</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B47" s="4">
         <v>12</v>
@@ -1638,9 +1639,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B48" s="4">
         <v>12</v>
@@ -1655,9 +1656,9 @@
         <v>51</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B49" s="4">
         <v>12</v>
@@ -1672,9 +1673,9 @@
         <v>52</v>
       </c>
     </row>
-    <row r="50" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B50" s="7">
         <v>13</v>
@@ -1687,9 +1688,9 @@
         <v>53</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B51" s="4">
         <v>13</v>
@@ -1704,9 +1705,9 @@
         <v>54</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B52" s="4">
         <v>13</v>
@@ -1721,9 +1722,9 @@
         <v>55</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B53" s="4">
         <v>13</v>
@@ -1738,7 +1739,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="55" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55"/>
       <c r="B55"/>
       <c r="C55"/>

</xml_diff>